<commit_message>
creating supplemental tables for lmm analysis of H1 and H2
</commit_message>
<xml_diff>
--- a/plots/SupplementalTable1.xlsx
+++ b/plots/SupplementalTable1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\AppraisingGrazing\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B787AE-E5B8-45AF-A1FA-F19B46D3FDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA75342-FC7F-4C09-800A-6B05BBDCA4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{BFB1EFBF-70C0-4387-B83F-E4C4F3BAF39A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>bison_1</t>
   </si>
@@ -81,24 +81,6 @@
     <t>untrtpd_3</t>
   </si>
   <si>
-    <t>bison/acre</t>
-  </si>
-  <si>
-    <t>cattle/acre</t>
-  </si>
-  <si>
-    <t>insecticide treatment</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>prairie dog presence</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -148,6 +130,81 @@
   </si>
   <si>
     <t>Blue Ridge, AP deeded</t>
+  </si>
+  <si>
+    <t>prairie dog dung/m2</t>
+  </si>
+  <si>
+    <t>17 ± 7.6 SE</t>
+  </si>
+  <si>
+    <t>6.7 ± 1.6 SE</t>
+  </si>
+  <si>
+    <t>11.6 ± 3.5 SE</t>
+  </si>
+  <si>
+    <t>6.3 ± 0.9 SE</t>
+  </si>
+  <si>
+    <t>156.1 ± 7 SE</t>
+  </si>
+  <si>
+    <t>15.8 ± 2.5 SE</t>
+  </si>
+  <si>
+    <t>8 ± 1.5 SE</t>
+  </si>
+  <si>
+    <t>6.2 ± 1.6 SE</t>
+  </si>
+  <si>
+    <t>6.4 ± 1.4 SE</t>
+  </si>
+  <si>
+    <t>9.6 ± 2 SE</t>
+  </si>
+  <si>
+    <t>6.5 ± 1.4 SE</t>
+  </si>
+  <si>
+    <t>15 ± 2.9 SE</t>
+  </si>
+  <si>
+    <t>7.4 ± 1.1 SE</t>
+  </si>
+  <si>
+    <t>3.5 ± 0.5 SE</t>
+  </si>
+  <si>
+    <t>2.3 ± 0.7 SE</t>
+  </si>
+  <si>
+    <t>0.8 ± 0.3 SE</t>
+  </si>
+  <si>
+    <t>1.1 ± 0.3 SE</t>
+  </si>
+  <si>
+    <t>1.8 ± 0.7 SE</t>
+  </si>
+  <si>
+    <t>7 ± 1.9 SE</t>
+  </si>
+  <si>
+    <t>10.9 ± 2.3 SE</t>
+  </si>
+  <si>
+    <t>19 ± 7.8 SE</t>
+  </si>
+  <si>
+    <t>cattle/ acre</t>
+  </si>
+  <si>
+    <t>bison/ acre</t>
+  </si>
+  <si>
+    <t>grasshoppers/ m2</t>
   </si>
 </sst>
 </file>
@@ -170,14 +227,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -225,26 +282,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -265,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +371,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +477,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,460 +635,461 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5">
+        <v>47.777996999999999</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-107.753106</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1.4448000000000001E-2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="7">
-        <v>47.777996999999999</v>
-      </c>
-      <c r="E2" s="7">
-        <v>-107.753106</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1.4448000000000001E-2</v>
-      </c>
-      <c r="G2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5">
         <v>47.977333000000002</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>-107.97136999999999</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>1.7616E-2</v>
       </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5">
         <v>47.897232000000002</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>-108.152952</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>1.2612999999999999E-2</v>
       </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7">
+        <v>47.754890000000003</v>
+      </c>
+      <c r="E5" s="7">
+        <v>-107.57931600000001</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2.4983999999999999E-2</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="8">
-        <v>47.754890000000003</v>
-      </c>
-      <c r="E5" s="8">
-        <v>-107.57931600000001</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>2.4983999999999999E-2</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>47.910995999999997</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>-108.05505700000001</v>
       </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
         <v>2.9739999999999999E-2</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7">
         <v>47.811923999999998</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>-108.175135</v>
       </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
         <v>2.63E-2</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>18</v>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5">
         <v>47.711489</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>-107.77458900000001</v>
       </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>18</v>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5">
         <v>47.697944999999997</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>-107.669584</v>
       </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5">
+        <v>48.391666999999998</v>
+      </c>
+      <c r="E10" s="5">
+        <v>-107.68186300000001</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="7">
-        <v>48.391666999999998</v>
-      </c>
-      <c r="E10" s="7">
-        <v>-107.68186300000001</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="7">
+        <v>47.781408999999996</v>
+      </c>
+      <c r="E11" s="7">
+        <v>-107.778515</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1.4448000000000001E-2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8">
-        <v>47.781408999999996</v>
-      </c>
-      <c r="E11" s="8">
-        <v>-107.778515</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="I11" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7">
+        <v>47.764141000000002</v>
+      </c>
+      <c r="E12" s="7">
+        <v>-107.746335</v>
+      </c>
+      <c r="F12" s="7">
         <v>1.4448000000000001E-2</v>
       </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="8">
-        <v>47.764141000000002</v>
-      </c>
-      <c r="E12" s="8">
-        <v>-107.746335</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="7">
+        <v>47.734526000000002</v>
+      </c>
+      <c r="E13" s="7">
+        <v>-107.77919900000001</v>
+      </c>
+      <c r="F13" s="7">
         <v>1.4448000000000001E-2</v>
       </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="8">
-        <v>47.734526000000002</v>
-      </c>
-      <c r="E13" s="8">
-        <v>-107.77919900000001</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1.4448000000000001E-2</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="B14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5">
         <v>47.982081999999998</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>-107.93881</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>1.7616E-2</v>
       </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="B15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="5">
         <v>47.893331000000003</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>-108.17267699999999</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <v>1.2612999999999999E-2</v>
       </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>36</v>
+      <c r="B16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="9">
         <v>47.870778000000001</v>
@@ -1037,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>